<commit_message>
update diary Duo Chai
</commit_message>
<xml_diff>
--- a/diaries/diary-Duo_Chai.xlsx
+++ b/diaries/diary-Duo_Chai.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="141">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -442,6 +442,15 @@
   </si>
   <si>
     <t>With the help of Soobin, we reviewed what we learnt from the classes, not that nervous about the final now.</t>
+  </si>
+  <si>
+    <t>17:00-20:40</t>
+  </si>
+  <si>
+    <t>Finished the 2nd issue PR</t>
+  </si>
+  <si>
+    <t>We figured out a solution to the 2nd issue while having a problem with our coding format through integration process. Our code works properly while the coding format doesn’t satisfy the TravisCi spotlessJava standard. We searched a lot of way to solve that problem but they all not working. Working together is also a key expert practice that we learnt from class and through the previous documentations of our assignments, we know that Glide team usually provides support in aligning code format and style. We decided to take the route of getting their help instead.</t>
   </si>
 </sst>
 </file>
@@ -2688,13 +2697,27 @@
       </c>
     </row>
     <row r="40" ht="15.5" customHeight="1">
-      <c r="A40" s="34"/>
-      <c r="B40" s="35"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="36"/>
+      <c r="A40" s="25">
+        <v>43906</v>
+      </c>
+      <c r="B40" t="s" s="20">
+        <v>138</v>
+      </c>
+      <c r="C40" t="s" s="20">
+        <v>34</v>
+      </c>
+      <c r="D40" t="s" s="20">
+        <v>131</v>
+      </c>
+      <c r="E40" t="s" s="20">
+        <v>139</v>
+      </c>
+      <c r="F40" t="s" s="20">
+        <v>140</v>
+      </c>
+      <c r="G40" t="s" s="24">
+        <v>20</v>
+      </c>
     </row>
     <row r="41" ht="15.5" customHeight="1">
       <c r="A41" s="34"/>

</xml_diff>